<commit_message>
tutorial level 2 complete
</commit_message>
<xml_diff>
--- a/docs/tasks/task_list.xlsx
+++ b/docs/tasks/task_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>Feature</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Save level to file</t>
   </si>
   <si>
@@ -232,6 +229,12 @@
   </si>
   <si>
     <t>Get time limit from level data</t>
+  </si>
+  <si>
+    <t>Init camera position at start of level</t>
+  </si>
+  <si>
+    <t>Init three.js objects</t>
   </si>
 </sst>
 </file>
@@ -456,8 +459,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -514,7 +519,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -534,6 +539,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -553,9 +559,10 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -613,146 +620,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1083,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G63"/>
+  <dimension ref="B1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1098,7 +965,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="23">
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="16" thickBot="1"/>
@@ -1127,7 +994,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="3">
@@ -1184,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1198,7 +1065,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1212,7 +1079,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1226,7 +1093,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1254,7 +1121,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1268,7 +1135,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1282,7 +1149,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1295,13 +1162,17 @@
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E15" s="3">
         <v>41183</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="3">
+        <v>41244</v>
+      </c>
       <c r="G15" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -1309,19 +1180,27 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="3">
+        <v>41276</v>
+      </c>
+      <c r="F16" s="3">
+        <v>41276</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1333,7 +1212,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1345,7 +1224,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1357,7 +1236,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1369,7 +1248,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1381,7 +1260,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1393,7 +1272,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1405,37 +1284,37 @@
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="3">
-        <v>41214</v>
-      </c>
-      <c r="F24" s="3">
-        <v>41214</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="7"/>
+      <c r="E25" s="3">
+        <v>41214</v>
+      </c>
+      <c r="F25" s="3">
+        <v>41214</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1447,7 +1326,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1459,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1471,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1483,7 +1362,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1491,20 +1370,20 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="6"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1515,7 +1394,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1527,7 +1406,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1539,7 +1418,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1551,7 +1430,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1563,7 +1442,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1575,7 +1454,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1587,7 +1466,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1599,7 +1478,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1611,7 +1490,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1623,7 +1502,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1635,7 +1514,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1647,7 +1526,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1659,7 +1538,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1671,7 +1550,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1683,7 +1562,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1695,7 +1574,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1707,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1719,7 +1598,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1731,7 +1610,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1739,57 +1618,67 @@
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="6"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="7"/>
+      <c r="E54" s="3">
+        <v>41276</v>
+      </c>
+      <c r="F54" s="3">
+        <v>41276</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="55" spans="2:7">
       <c r="B55" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="7"/>
+      <c r="E55" s="3">
+        <v>41277</v>
+      </c>
+      <c r="F55" s="3">
+        <v>41278</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="56" spans="2:7">
       <c r="B56" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1798,10 +1687,10 @@
     </row>
     <row r="57" spans="2:7">
       <c r="B57" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -1810,10 +1699,10 @@
     </row>
     <row r="58" spans="2:7">
       <c r="B58" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -1822,7 +1711,7 @@
     </row>
     <row r="59" spans="2:7">
       <c r="B59" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>55</v>
@@ -1834,10 +1723,10 @@
     </row>
     <row r="60" spans="2:7">
       <c r="B60" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1846,10 +1735,10 @@
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1858,50 +1747,62 @@
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="2:7" ht="16" thickBot="1">
-      <c r="B63" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="10"/>
+    <row r="63" spans="2:7">
+      <c r="B63" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="2:7" ht="16" thickBot="1">
+      <c r="B64" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G5)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="6" priority="4" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="4" priority="4" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G5))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G9 G11:G63">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Done">
+  <conditionalFormatting sqref="G4:G9 G11:G64">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G4)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="4" priority="6" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="2" priority="6" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G10)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="2" priority="2" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="0" priority="2" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G10))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
completed tutorial level4 - rotate view
</commit_message>
<xml_diff>
--- a/docs/tasks/task_list.xlsx
+++ b/docs/tasks/task_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="77">
   <si>
     <t>Feature</t>
   </si>
@@ -180,33 +180,12 @@
     <t>Level 4 - rotate view to complete level</t>
   </si>
   <si>
-    <t>Level 5 - can fall off level and die</t>
-  </si>
-  <si>
-    <t>Level 7 - moving enemy</t>
-  </si>
-  <si>
-    <t>Level 6 - moving blocks</t>
-  </si>
-  <si>
-    <t>Level 8 - moving enemy &amp; blocks</t>
-  </si>
-  <si>
-    <t>Level 9 - level contains trigger switch to start movement</t>
-  </si>
-  <si>
-    <t>Level 10 - level contains trigger switch to enable light</t>
-  </si>
-  <si>
     <t>If play hits switch animation starts/stops</t>
   </si>
   <si>
     <t>If play hits switch light on/off</t>
   </si>
   <si>
-    <t>Level 11 - multiple balls on level</t>
-  </si>
-  <si>
     <t>A2B.js Task list</t>
   </si>
   <si>
@@ -235,13 +214,49 @@
   </si>
   <si>
     <t>Init three.js objects</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Play Level</t>
+  </si>
+  <si>
+    <t>Weird square shadown on top of block on level 4</t>
+  </si>
+  <si>
+    <t>Amended shadow parms on camera in level4.json</t>
+  </si>
+  <si>
+    <t>Level 6 - can fall off level and die</t>
+  </si>
+  <si>
+    <t>Level 7 - moving blocks</t>
+  </si>
+  <si>
+    <t>Level 8 - moving enemy</t>
+  </si>
+  <si>
+    <t>Level 9 - moving enemy &amp; blocks</t>
+  </si>
+  <si>
+    <t>Level 10 - level contains trigger switch to start movement</t>
+  </si>
+  <si>
+    <t>Level 11 - level contains trigger switch to enable light</t>
+  </si>
+  <si>
+    <t>Level 12 - multiple balls on level</t>
+  </si>
+  <si>
+    <t>Level 5 - can run out of time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -294,6 +309,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -459,7 +481,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -501,8 +523,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -518,8 +546,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -540,6 +570,9 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -560,9 +593,92 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -950,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G64"/>
+  <dimension ref="B1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -965,7 +1081,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="23">
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="16" thickBot="1"/>
@@ -1051,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1065,7 +1181,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1079,7 +1195,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1093,7 +1209,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1121,7 +1237,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1135,7 +1251,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1149,7 +1265,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1163,7 +1279,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E15" s="3">
         <v>41183</v>
@@ -1183,7 +1299,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E16" s="3">
         <v>41276</v>
@@ -1362,7 +1478,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1374,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1681,9 +1797,15 @@
         <v>51</v>
       </c>
       <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="7"/>
+      <c r="E56" s="3">
+        <v>41278</v>
+      </c>
+      <c r="F56" s="3">
+        <v>41278</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="57" spans="2:7">
       <c r="B57" s="6" t="s">
@@ -1693,16 +1815,22 @@
         <v>52</v>
       </c>
       <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="7"/>
+      <c r="E57" s="3">
+        <v>41281</v>
+      </c>
+      <c r="F57" s="3">
+        <v>41281</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="58" spans="2:7">
       <c r="B58" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -1713,8 +1841,8 @@
       <c r="B59" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>55</v>
+      <c r="C59" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -1726,7 +1854,7 @@
         <v>48</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1738,7 +1866,7 @@
         <v>48</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1750,7 +1878,7 @@
         <v>48</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1762,48 +1890,101 @@
         <v>48</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="2:7" ht="16" thickBot="1">
-      <c r="B64" s="8" t="s">
+    <row r="64" spans="2:7">
+      <c r="B64" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C64" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="10"/>
+      <c r="C64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="2:7" ht="16" thickBot="1">
+      <c r="B65" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="10"/>
+    </row>
+    <row r="67" spans="2:7" ht="20">
+      <c r="B67" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="16" thickBot="1">
+      <c r="B68" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E68" s="15">
+        <v>41281</v>
+      </c>
+      <c r="F68" s="15">
+        <v>41281</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G5)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="4" priority="4" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="10" priority="8" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G5))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G9 G11:G64">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Done">
+  <conditionalFormatting sqref="G4:G9 G11:G58 G60:G65">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G4)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="2" priority="6" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="8" priority="10" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G10)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="0" priority="2" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="6" priority="6" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G10))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G68">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",G68)))</formula>
+    </cfRule>
+    <cfRule type="notContainsText" dxfId="4" priority="4" operator="notContains" text="Done">
+      <formula>ISERROR(SEARCH("Done",G68))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G59">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",G59)))</formula>
+    </cfRule>
+    <cfRule type="notContainsText" dxfId="2" priority="2" operator="notContains" text="Done">
+      <formula>ISERROR(SEARCH("Done",G59))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changed the "lookat" position of of the camera to be near the origin to make the rotation feel more natural
</commit_message>
<xml_diff>
--- a/docs/tasks/task_list.xlsx
+++ b/docs/tasks/task_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
   <si>
     <t>Feature</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Level 5 - can run out of time</t>
+  </si>
+  <si>
+    <t>Display score &amp; time on HUD</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -548,6 +551,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1066,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G68"/>
+  <dimension ref="B1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1442,10 +1448,12 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="3">
+        <v>41281</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="7"/>
     </row>
@@ -1454,7 +1462,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1466,7 +1474,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1478,7 +1486,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1490,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1498,20 +1506,20 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="6"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1522,7 +1530,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1534,7 +1542,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1546,7 +1554,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1558,7 +1566,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1570,7 +1578,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1582,7 +1590,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1594,7 +1602,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1606,7 +1614,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1618,7 +1626,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1630,7 +1638,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1642,7 +1650,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1654,7 +1662,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1666,7 +1674,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1678,7 +1686,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1690,7 +1698,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1702,7 +1710,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1714,7 +1722,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1726,7 +1734,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1738,7 +1746,7 @@
         <v>4</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1746,44 +1754,38 @@
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="6"/>
-      <c r="C53" s="2"/>
+      <c r="B53" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="7"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="3">
-        <v>41276</v>
-      </c>
-      <c r="F54" s="3">
-        <v>41276</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="7"/>
     </row>
     <row r="55" spans="2:7">
       <c r="B55" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="3">
-        <v>41277</v>
+        <v>41276</v>
       </c>
       <c r="F55" s="3">
-        <v>41278</v>
+        <v>41276</v>
       </c>
       <c r="G55" s="7" t="s">
         <v>27</v>
@@ -1794,11 +1796,11 @@
         <v>48</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="3">
-        <v>41278</v>
+        <v>41277</v>
       </c>
       <c r="F56" s="3">
         <v>41278</v>
@@ -1812,14 +1814,14 @@
         <v>48</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="3">
-        <v>41281</v>
+        <v>41278</v>
       </c>
       <c r="F57" s="3">
-        <v>41281</v>
+        <v>41278</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>27</v>
@@ -1829,20 +1831,26 @@
       <c r="B58" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>76</v>
+      <c r="C58" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="7"/>
+      <c r="E58" s="3">
+        <v>41281</v>
+      </c>
+      <c r="F58" s="3">
+        <v>41281</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="59" spans="2:7">
       <c r="B59" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -1853,8 +1861,8 @@
       <c r="B60" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>70</v>
+      <c r="C60" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1866,7 +1874,7 @@
         <v>48</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1878,7 +1886,7 @@
         <v>48</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1890,7 +1898,7 @@
         <v>48</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1902,89 +1910,101 @@
         <v>48</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="2:7" ht="16" thickBot="1">
-      <c r="B65" s="8" t="s">
+    <row r="65" spans="2:7">
+      <c r="B65" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="7"/>
+    </row>
+    <row r="66" spans="2:7" ht="16" thickBot="1">
+      <c r="B66" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="10"/>
-    </row>
-    <row r="67" spans="2:7" ht="20">
-      <c r="B67" s="16" t="s">
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="10"/>
+    </row>
+    <row r="68" spans="2:7" ht="20">
+      <c r="B68" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="2:7" ht="16" thickBot="1">
-      <c r="B68" s="8" t="s">
+    <row r="69" spans="2:7" ht="31" thickBot="1">
+      <c r="B69" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C69" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D69" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E68" s="15">
+      <c r="E69" s="15">
         <v>41281</v>
       </c>
-      <c r="F68" s="15">
+      <c r="F69" s="15">
         <v>41281</v>
       </c>
-      <c r="G68" s="10" t="s">
+      <c r="G69" s="10" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G5)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="10" priority="8" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="8" priority="8" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G5))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G9 G11:G58 G60:G65">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Done">
+  <conditionalFormatting sqref="G4:G9 G11:G59 G61:G66">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G4)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="8" priority="10" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="6" priority="10" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G10)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="6" priority="6" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="4" priority="6" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G10))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G68">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",G68)))</formula>
+  <conditionalFormatting sqref="G69">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",G69)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="4" priority="4" operator="notContains" text="Done">
-      <formula>ISERROR(SEARCH("Done",G68))</formula>
+    <cfRule type="notContainsText" dxfId="2" priority="4" operator="notContains" text="Done">
+      <formula>ISERROR(SEARCH("Done",G69))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G59">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",G59)))</formula>
+  <conditionalFormatting sqref="G60">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",G60)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="2" priority="2" operator="notContains" text="Done">
-      <formula>ISERROR(SEARCH("Done",G59))</formula>
+    <cfRule type="notContainsText" dxfId="0" priority="2" operator="notContains" text="Done">
+      <formula>ISERROR(SEARCH("Done",G60))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
level timeLimit from json files
</commit_message>
<xml_diff>
--- a/docs/tasks/task_list.xlsx
+++ b/docs/tasks/task_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
   <si>
     <t>Feature</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Display score &amp; time on HUD</t>
+  </si>
+  <si>
+    <t>camera rotation didn't feel natural</t>
+  </si>
+  <si>
+    <t>moved lookat position to origin</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -532,8 +538,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -554,8 +570,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -579,6 +607,11 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -602,9 +635,34 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1072,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G69"/>
+  <dimension ref="B1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1941,70 +1999,232 @@
       <c r="F66" s="9"/>
       <c r="G66" s="10"/>
     </row>
-    <row r="68" spans="2:7" ht="20">
+    <row r="67" spans="2:7">
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+    </row>
+    <row r="68" spans="2:7" ht="21" thickBot="1">
       <c r="B68" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="2:7" ht="31" thickBot="1">
-      <c r="B69" s="8" t="s">
+    <row r="69" spans="2:7" ht="30">
+      <c r="B69" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D69" s="17" t="s">
+      <c r="D69" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="E69" s="15">
+      <c r="E69" s="24">
         <v>41281</v>
       </c>
-      <c r="F69" s="15">
+      <c r="F69" s="24">
         <v>41281</v>
       </c>
-      <c r="G69" s="10" t="s">
+      <c r="G69" s="25" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E70" s="3">
+        <v>41319</v>
+      </c>
+      <c r="F70" s="3">
+        <v>41319</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" s="6"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="7"/>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" s="6"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="7"/>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="B73" s="6"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74" s="6"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="7"/>
+    </row>
+    <row r="75" spans="2:7">
+      <c r="B75" s="6"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="2:7">
+      <c r="B76" s="6"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="7"/>
+    </row>
+    <row r="77" spans="2:7">
+      <c r="B77" s="6"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78" spans="2:7">
+      <c r="B78" s="6"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="7"/>
+    </row>
+    <row r="79" spans="2:7">
+      <c r="B79" s="6"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="7"/>
+    </row>
+    <row r="80" spans="2:7">
+      <c r="B80" s="6"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="7"/>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81" s="6"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="7"/>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82" s="6"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="7"/>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" s="6"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="7"/>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" s="6"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="7"/>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85" s="6"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="7"/>
+    </row>
+    <row r="86" spans="2:7" ht="16" thickBot="1">
+      <c r="B86" s="8"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G5)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="8" priority="8" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="14" priority="10" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G9 G11:G59 G61:G66">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G4)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="6" priority="10" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="12" priority="12" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G10)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="4" priority="6" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="10" priority="8" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G69">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G69)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="2" priority="4" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="8" priority="6" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G69))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G60)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="0" priority="2" operator="notContains" text="Done">
+    <cfRule type="notContainsText" dxfId="6" priority="4" operator="notContains" text="Done">
       <formula>ISERROR(SEARCH("Done",G60))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G70:G86">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",G70)))</formula>
+    </cfRule>
+    <cfRule type="notContainsText" dxfId="4" priority="2" operator="notContains" text="Done">
+      <formula>ISERROR(SEARCH("Done",G70))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
play now dies when time runs out, until all lives used
</commit_message>
<xml_diff>
--- a/docs/tasks/task_list.xlsx
+++ b/docs/tasks/task_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
   <si>
     <t>Feature</t>
   </si>
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1261,9 +1261,15 @@
       <c r="D9" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="14"/>
+      <c r="E9" s="3">
+        <v>41320</v>
+      </c>
+      <c r="F9" s="3">
+        <v>41320</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="6" t="s">
@@ -1275,9 +1281,15 @@
       <c r="D10" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="14"/>
+      <c r="E10" s="3">
+        <v>41320</v>
+      </c>
+      <c r="F10" s="3">
+        <v>41320</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="6" t="s">
@@ -1289,9 +1301,15 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="14"/>
+      <c r="E11" s="3">
+        <v>41320</v>
+      </c>
+      <c r="F11" s="3">
+        <v>41320</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="6" t="s">
@@ -1512,8 +1530,12 @@
       <c r="E27" s="3">
         <v>41281</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="7"/>
+      <c r="F27" s="3">
+        <v>41319</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="2:7">
       <c r="B28" s="6" t="s">

</xml_diff>

<commit_message>
player dies if they fall off platform
</commit_message>
<xml_diff>
--- a/docs/tasks/task_list.xlsx
+++ b/docs/tasks/task_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="80">
   <si>
     <t>Feature</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Play Level</t>
   </si>
   <si>
-    <t>Weird square shadown on top of block on level 4</t>
-  </si>
-  <si>
     <t>Amended shadow parms on camera in level4.json</t>
   </si>
   <si>
@@ -259,6 +256,9 @@
   </si>
   <si>
     <t>moved lookat position to origin</t>
+  </si>
+  <si>
+    <t>Weird square shadow on top of block on level 4</t>
   </si>
 </sst>
 </file>
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1524,7 +1524,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="3">
@@ -1930,19 +1930,25 @@
         <v>48</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="7"/>
+      <c r="E59" s="3">
+        <v>41320</v>
+      </c>
+      <c r="F59" s="3">
+        <v>41320</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="60" spans="2:7">
       <c r="B60" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1954,7 +1960,7 @@
         <v>48</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1966,7 +1972,7 @@
         <v>48</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1978,7 +1984,7 @@
         <v>48</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1990,7 +1996,7 @@
         <v>48</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -2002,7 +2008,7 @@
         <v>48</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -2014,7 +2020,7 @@
         <v>48</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
@@ -2037,10 +2043,10 @@
         <v>66</v>
       </c>
       <c r="C69" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="23" t="s">
         <v>67</v>
-      </c>
-      <c r="D69" s="23" t="s">
-        <v>68</v>
       </c>
       <c r="E69" s="24">
         <v>41281</v>
@@ -2057,10 +2063,10 @@
         <v>66</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D70" s="20" t="s">
         <v>78</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>79</v>
       </c>
       <c r="E70" s="3">
         <v>41319</v>

</xml_diff>

<commit_message>
added tutorial level six, don't fall off the platforms
</commit_message>
<xml_diff>
--- a/docs/tasks/task_list.xlsx
+++ b/docs/tasks/task_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="80">
   <si>
     <t>Feature</t>
   </si>
@@ -180,12 +180,6 @@
     <t>Level 4 - rotate view to complete level</t>
   </si>
   <si>
-    <t>If play hits switch animation starts/stops</t>
-  </si>
-  <si>
-    <t>If play hits switch light on/off</t>
-  </si>
-  <si>
     <t>A2B.js Task list</t>
   </si>
   <si>
@@ -259,6 +253,12 @@
   </si>
   <si>
     <t>Weird square shadow on top of block on level 4</t>
+  </si>
+  <si>
+    <t>If player hits switch animation starts/stops</t>
+  </si>
+  <si>
+    <t>If player hits switch light on/off</t>
   </si>
 </sst>
 </file>
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1145,7 +1145,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="23">
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="16" thickBot="1"/>
@@ -1231,11 +1231,17 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="14"/>
+        <v>55</v>
+      </c>
+      <c r="E7" s="3">
+        <v>41320</v>
+      </c>
+      <c r="F7" s="3">
+        <v>41320</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="6" t="s">
@@ -1245,11 +1251,17 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="14"/>
+        <v>54</v>
+      </c>
+      <c r="E8" s="3">
+        <v>41320</v>
+      </c>
+      <c r="F8" s="3">
+        <v>41320</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="6" t="s">
@@ -1259,7 +1271,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3">
         <v>41320</v>
@@ -1279,7 +1291,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="3">
         <v>41320</v>
@@ -1319,7 +1331,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1333,7 +1345,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1347,7 +1359,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1361,7 +1373,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="3">
         <v>41183</v>
@@ -1381,7 +1393,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="3">
         <v>41276</v>
@@ -1524,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="3">
@@ -1578,7 +1590,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1590,7 +1602,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1930,7 +1942,7 @@
         <v>48</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="3">
@@ -1948,19 +1960,25 @@
         <v>48</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="7"/>
+      <c r="E60" s="3">
+        <v>41320</v>
+      </c>
+      <c r="F60" s="3">
+        <v>41320</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1972,7 +1990,7 @@
         <v>48</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1984,7 +2002,7 @@
         <v>48</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1996,7 +2014,7 @@
         <v>48</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -2008,7 +2026,7 @@
         <v>48</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -2020,7 +2038,7 @@
         <v>48</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
@@ -2035,18 +2053,18 @@
     </row>
     <row r="68" spans="2:7" ht="21" thickBot="1">
       <c r="B68" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="30">
       <c r="B69" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E69" s="24">
         <v>41281</v>
@@ -2060,13 +2078,13 @@
     </row>
     <row r="70" spans="2:7">
       <c r="B70" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E70" s="3">
         <v>41319</v>

</xml_diff>